<commit_message>
Model training severe changes
</commit_message>
<xml_diff>
--- a/resources/experiment 1/metrics/MAPE/average time/Amputación extremidades inferiores.xlsx
+++ b/resources/experiment 1/metrics/MAPE/average time/Amputación extremidades inferiores.xlsx
@@ -478,45 +478,45 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.009851869966974741</v>
+        <v>0.009183249939904782</v>
       </c>
       <c r="C3" t="n">
-        <v>0.009851869966974741</v>
+        <v>0.01005644336237487</v>
       </c>
       <c r="D3" t="n">
-        <v>0.009851869966974741</v>
+        <v>0.01096883779990067</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>GradientBoostingRegressor</t>
+          <t>DecisionTreeRegressor</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.008122682715386874</v>
+        <v>0.008486287632614541</v>
       </c>
       <c r="C4" t="n">
-        <v>0.008122682715386874</v>
+        <v>0.008424325166877212</v>
       </c>
       <c r="D4" t="n">
-        <v>0.008122682715386874</v>
+        <v>0.008501509040853873</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>AdaBoostRegressor</t>
+          <t>MLPRegressor</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.02978680454395516</v>
+        <v>0.009254582960705032</v>
       </c>
       <c r="C5" t="n">
-        <v>0.02978680454395516</v>
+        <v>0.009179242514751428</v>
       </c>
       <c r="D5" t="n">
-        <v>0.02978680454395516</v>
+        <v>0.008666441091175241</v>
       </c>
     </row>
   </sheetData>

</xml_diff>